<commit_message>
Towards a generalized data model extraction
</commit_message>
<xml_diff>
--- a/output/data_model.xlsx
+++ b/output/data_model.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -831,19 +831,19 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>{'Komorbiditet kategori': 'Fordøyelsessystemet, sykdommer (Kap.XI; K00-K93)', 'Komorbiditet tilstand': 'Psykiske lidelser og atferdsforstyrrelser (Kap.V; F00-F99)', 'ICD10 tilstand': 'diam tincidunt erat martine ipsum nibh lars. gjøran aliquam gøran martine magna nibh aliquam bjørn øystein diam nonummy consectetuer consectetuer. martine sit ipsum gøran sed erat runar sit nibh. diam nonummy bjørn dolore adipiscing consectetuer nonummy tincidunt diam euismod.'}</t>
+          <t>{'Sykdomskategori': 'Fordøyelsessystemet, sykdommer (Kap.XI; K00-K93)', 'Sykdomstilstand': 'Psykiske lidelser og atferdsforstyrrelser (Kap.V; F00-F99)'}</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>seneffekter</t>
+          <t>komorbiditet</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kategori</t>
+          <t>ICD10 symbol</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -851,19 +851,19 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Blood and lymphatic system disorders</t>
+          <t>diam tincidunt erat marti....</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>seneffekter</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Term</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -871,379 +871,379 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>{'Kategori': 'Aldersgruppe', 'Verdi': '1', 'Symbol': '50-59 år'}</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>seneffekter</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Grad</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>{'Kategori': 'Myokardinfarkt', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>seneffekter</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Grad symbol</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Grad 0</t>
+          <t>{'Kategori': 'Kronisk hjertesvikt', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>seneffekter</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Beskrivelse av grad</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>{'Kategori': 'Perifere vaskulære sykdommer', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>seneffekter</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>CTCAE versjon</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>team selecta diam gjøran ....</t>
+          <t>{'Kategori': 'Cerebrovaskulær hendelse', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>diagnose</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>bjørn amet euismod euismo....</t>
+          <t>{'Kategori': 'Demens', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Anatomisk lokalisering</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Begge</t>
+          <t>{'Kategori': 'Kronisk lungesykdom', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Dato/tid for klinisk bekreftelse</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2024-11-18T22:55:53.3652492+01:00</t>
+          <t>{'Kategori': 'Ulcussykdom', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Multiple primærtumorer</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Multiple primærtumorer</t>
+          <t>{'Kategori': 'Leversykdom', 'Verdi': '0', 'Symbol': 'Ingen'}</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Klinisk T</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>cT0</t>
+          <t>{'Kategori': 'Bindevevssykdom', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Klinisk N</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>cN1b</t>
+          <t>{'Kategori': 'Diabetes', 'Verdi': '0', 'Symbol': 'Ingen eller diettkontrollert'}</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Klinisk M</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>cM0</t>
+          <t>{'Kategori': 'Hemiplegi', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Klinisk residiv</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>{'Kategori': 'Moderat til alvorlig nyresykdom', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Klinisk TNM-vurdering</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>runar bjørn diam gjøran m....</t>
+          <t>{'Kategori': 'Solid svulst', 'Verdi': '0', 'Symbol': 'Ingen'}</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Klinisk TNM-utgave</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>AJCC TNM Versjon 8</t>
+          <t>{'Kategori': 'Leukemi', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Patologisk T</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>pT4b</t>
+          <t>{'Kategori': 'Lymfom', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Patologisk N</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>pN1</t>
+          <t>{'Kategori': 'AIDS', 'Verdi': '0', 'Symbol': 'Nei'}</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Patologisk M</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>pM0</t>
+          <t>{'Kategori': 'CCI totalskår', 'Verdi': '82'}</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>CCI</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Patologisk residiv</t>
+          <t>items</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>{'Kategori': 'Estimert overlevelse etter 10 år', 'Verdi': '82', 'Enhet': '%'}</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>seneffekter</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Patologisk TNM-vurdering</t>
+          <t>Kategori</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1251,19 +1251,19 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>gøran euismod sed kjetil ....</t>
+          <t>Blood and lymphatic system disorders</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>primærdiagnose</t>
+          <t>seneffekter</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Patologisk TNM-utgave</t>
+          <t>Term</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1271,19 +1271,19 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>AJCC TNM Versjon 8</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>lymeknutemetastase</t>
+          <t>seneffekter</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Regional lymfeknutemetastase</t>
+          <t>Grad</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1291,19 +1291,19 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Reginoale lymfeknutemetastase</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>lymeknutemetastase</t>
+          <t>seneffekter</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Metode</t>
+          <t>Grad symbol</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1311,19 +1311,19 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Annet</t>
+          <t>Grad 0</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>lymeknutemetastase</t>
+          <t>seneffekter</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Funn</t>
+          <t>Beskrivelse av grad</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1331,19 +1331,19 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Reginoale lymfeknutemetastase</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>fjernmetastaser</t>
+          <t>seneffekter</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Fjernmetastaser</t>
+          <t>CTCAE versjon</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1351,19 +1351,19 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Fjernmetastase</t>
+          <t>team selecta diam gjøran ....</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>fjernmetastaser</t>
+          <t>primærdiagnose</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Funn</t>
+          <t>diagnose</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1371,19 +1371,19 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Fjernmetastase</t>
+          <t>bjørn amet euismod euismo....</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>fjernmetastaser</t>
+          <t>primærdiagnose</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Metode</t>
+          <t>Anatomisk lokalisering</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1391,19 +1391,19 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Reseksjon</t>
+          <t>Begge</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>fjernmetastaser</t>
+          <t>primærdiagnose</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Anatomisk lokalisasjon</t>
+          <t>Dato/tid for klinisk bekreftelse</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1411,119 +1411,119 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Skjelett</t>
+          <t>2024-11-18T22:55:53.3652492+01:00</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>fjernmetastaser</t>
+          <t>primærdiagnose</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Anatomisk lokalisasjon</t>
+          <t>Multiple primærtumorer</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Lever</t>
+          <t>Multiple primærtumorer</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>fjernmetastaser</t>
+          <t>primærdiagnose</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Anatomisk lokalisasjon</t>
+          <t>Klinisk T</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Lunge</t>
+          <t>cT0</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>fjernmetastaser</t>
+          <t>primærdiagnose</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Anatomisk lokalisasjon</t>
+          <t>Klinisk N</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>CNS (sentralnervesystemet)</t>
+          <t>cN1b</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>fjernmetastaser</t>
+          <t>primærdiagnose</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Anatomisk lokalisasjon</t>
+          <t>Klinisk M</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>dolore dolor adipiscing a....</t>
+          <t>cM0</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>fjernmetastaser</t>
+          <t>primærdiagnose</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Anatomisk lokalisasjon</t>
+          <t>Klinisk residiv</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>diam gøran tincidunt sed ....</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>ECOG</t>
+          <t>primærdiagnose</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ECOG verdi</t>
+          <t>Klinisk TNM-vurdering</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1531,19 +1531,19 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>runar bjørn diam gjøran m....</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>ECOG</t>
+          <t>primærdiagnose</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ECOG symbol</t>
+          <t>Klinisk TNM-utgave</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1551,25 +1551,425 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Symptomatisk, fullt oppegående</t>
+          <t>AJCC TNM Versjon 8</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>primærdiagnose</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Patologisk T</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>pT4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>primærdiagnose</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Patologisk N</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>pN1</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>primærdiagnose</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Patologisk M</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>pM0</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>primærdiagnose</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Patologisk residiv</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>primærdiagnose</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Patologisk TNM-vurdering</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>gøran euismod sed kjetil ....</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>primærdiagnose</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Patologisk TNM-utgave</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>AJCC TNM Versjon 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>lymeknutemetastase</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Regional lymfeknutemetastase</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Reginoale lymfeknutemetastase</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>lymeknutemetastase</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Metode</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Annet</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>lymeknutemetastase</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Funn</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Reginoale lymfeknutemetastase</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>fjernmetastaser</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Fjernmetastaser</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Fjernmetastase</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>fjernmetastaser</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Funn</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Fjernmetastase</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>fjernmetastaser</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Metode</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>1</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Reseksjon</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>fjernmetastaser</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Anatomisk lokalisasjon</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Skjelett</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>fjernmetastaser</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Anatomisk lokalisasjon</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>2</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Lever</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>fjernmetastaser</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Anatomisk lokalisasjon</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>3</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Lunge</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>fjernmetastaser</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Anatomisk lokalisasjon</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>4</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>CNS (sentralnervesystemet)</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>fjernmetastaser</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Anatomisk lokalisasjon</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>5</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>dolore dolor adipiscing a....</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>fjernmetastaser</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Anatomisk lokalisasjon</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>6</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>diam gøran tincidunt sed ....</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
           <t>ECOG</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ECOG verdi</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>1</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>ECOG</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>ECOG symbol</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>1</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Symptomatisk, fullt oppegående</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>ECOG</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
         <is>
           <t>ECOG tidspunkt</t>
         </is>
       </c>
-      <c r="C57" t="n">
-        <v>1</v>
-      </c>
-      <c r="D57" t="inlineStr">
+      <c r="C77" t="n">
+        <v>1</v>
+      </c>
+      <c r="D77" t="inlineStr">
         <is>
           <t>2024-10-22T03:55:53.3426975+02:00</t>
         </is>

</xml_diff>